<commit_message>
Making changes to Lab 19.
</commit_message>
<xml_diff>
--- a/19_anemia/19_anemia_data.xlsx
+++ b/19_anemia/19_anemia_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Anemia Data</t>
   </si>
@@ -64,6 +64,45 @@
   </si>
   <si>
     <t>Cardiac Output(mL/min)</t>
+  </si>
+  <si>
+    <t>Exercise Data</t>
+  </si>
+  <si>
+    <t>0’</t>
+  </si>
+  <si>
+    <t>1’</t>
+  </si>
+  <si>
+    <t>2’</t>
+  </si>
+  <si>
+    <t>3’</t>
+  </si>
+  <si>
+    <t>4’</t>
+  </si>
+  <si>
+    <t>5’</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Heart Rate</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Elapsed Time (Min)</t>
+  </si>
+  <si>
+    <t>Distance Traveled (Ft)</t>
   </si>
 </sst>
 </file>
@@ -93,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -149,11 +188,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -167,10 +234,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -467,24 +552,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:I7"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="5" t="s">
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -496,7 +584,7 @@
       <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="1">
@@ -508,9 +596,30 @@
       <c r="I2" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A3" s="6"/>
+      <c r="K2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -520,7 +629,7 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
@@ -530,8 +639,29 @@
       <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="60.75" thickBot="1">
+      <c r="K3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>6</v>
+      </c>
+      <c r="N3" s="2">
+        <v>6</v>
+      </c>
+      <c r="O3" s="2">
+        <v>6</v>
+      </c>
+      <c r="P3" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="60.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -556,8 +686,29 @@
       <c r="I4" s="4">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="45.75" thickBot="1">
+      <c r="K4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="10">
+        <v>0</v>
+      </c>
+      <c r="M4" s="10">
+        <v>0</v>
+      </c>
+      <c r="N4" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="O4" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="P4" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="45.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -582,8 +733,29 @@
       <c r="I5" s="4">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="30.75" thickBot="1">
+      <c r="K5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="4">
+        <v>87</v>
+      </c>
+      <c r="M5" s="4">
+        <v>126</v>
+      </c>
+      <c r="N5" s="4">
+        <v>137</v>
+      </c>
+      <c r="O5" s="4">
+        <v>155</v>
+      </c>
+      <c r="P5" s="4">
+        <v>152</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="30.75" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -596,20 +768,20 @@
       <c r="D6" s="4">
         <v>27</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>5361</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="6">
         <v>6149</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="6">
         <v>6944</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45.75" thickBot="1">
+    <row r="7" spans="1:17" ht="45.75" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -622,12 +794,18 @@
       <c r="D7" s="4">
         <v>0.12</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="45.75" thickBot="1">
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="K7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="12">
+        <v>0.21944444444444444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="60.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -640,8 +818,14 @@
       <c r="D8" s="4">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="45.75" thickBot="1">
+      <c r="K8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="8">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="45.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -655,7 +839,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45.75" thickBot="1">
+    <row r="10" spans="1:17" ht="45.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -669,7 +853,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="75.75" thickBot="1">
+    <row r="11" spans="1:17" ht="75.75" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -685,12 +869,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Lab 19 HumMod data, it cannot be completed.
</commit_message>
<xml_diff>
--- a/19_anemia/19_anemia_data.xlsx
+++ b/19_anemia/19_anemia_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
   <si>
     <t>Anemia Data</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Exercise was started after two months.</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>This lab cannot be completed at the moment because red cell production cannot be changed in HumMod</t>
   </si>
 </sst>
 </file>
@@ -235,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -268,13 +277,22 @@
       <alignment horizontal="left" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,27 +587,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="S7" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" thickBot="1">
+    <row r="1" spans="1:36" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
       <c r="F1" t="s">
         <v>13</v>
       </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
       <c r="K1" t="s">
         <v>16</v>
       </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:36" ht="15.75" thickBot="1">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -601,7 +646,7 @@
       <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="1">
@@ -634,9 +679,54 @@
       <c r="Q2" s="6" t="s">
         <v>22</v>
       </c>
+      <c r="T2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A3" s="13"/>
+    <row r="3" spans="1:36" ht="15.75" thickBot="1">
+      <c r="A3" s="15"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -646,7 +736,7 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="13"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
@@ -677,8 +767,49 @@
       <c r="Q3" s="2">
         <v>6</v>
       </c>
+      <c r="T3" s="15"/>
+      <c r="U3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>6</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>6</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>6</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>6</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" ht="60.75" thickBot="1">
+    <row r="4" spans="1:36" ht="60.75" thickBot="1">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -724,8 +855,43 @@
       <c r="Q4" s="7">
         <v>0.08</v>
       </c>
+      <c r="T4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" s="3">
+        <v>2340</v>
+      </c>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="Y4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AD4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE4" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="AH4" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="AI4" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="AJ4" s="7">
+        <v>0.08</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" ht="45.75" thickBot="1">
+    <row r="5" spans="1:36" ht="45.75" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -771,8 +937,31 @@
       <c r="Q5" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="T5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="U5" s="3">
+        <v>3081</v>
+      </c>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="Y5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AD5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
     </row>
-    <row r="6" spans="1:21" ht="30.75" customHeight="1" thickBot="1">
+    <row r="6" spans="1:36" ht="30.75" customHeight="1" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -785,16 +974,16 @@
       <c r="D6" s="3">
         <v>27</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="14">
         <v>5346</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="14">
         <v>5901</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="14">
         <v>6849</v>
       </c>
       <c r="K6" s="10" t="s">
@@ -804,14 +993,35 @@
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="U6" s="3">
+        <v>43</v>
+      </c>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="Y6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
+      <c r="AD6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
     </row>
-    <row r="7" spans="1:21" ht="45.75" thickBot="1">
+    <row r="7" spans="1:36" ht="45.75" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -824,18 +1034,34 @@
       <c r="D7" s="3">
         <v>0.12</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
       <c r="K7" s="8" t="s">
         <v>27</v>
       </c>
       <c r="L7" s="9">
         <v>0.1763888888888889</v>
       </c>
+      <c r="T7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0.192</v>
+      </c>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="15"/>
+      <c r="AD7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE7" s="9"/>
     </row>
-    <row r="8" spans="1:21" ht="60.75" thickBot="1">
+    <row r="8" spans="1:36" ht="60.75" thickBot="1">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -854,8 +1080,20 @@
       <c r="L8" s="5">
         <v>2236</v>
       </c>
+      <c r="T8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="U8" s="3">
+        <v>92.6</v>
+      </c>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="AD8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE8" s="5"/>
     </row>
-    <row r="9" spans="1:21" ht="45.75" thickBot="1">
+    <row r="9" spans="1:36" ht="45.75" thickBot="1">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -868,8 +1106,16 @@
       <c r="D9" s="3">
         <v>0.08</v>
       </c>
+      <c r="T9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="U9" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:21" ht="45.75" thickBot="1">
+    <row r="10" spans="1:36" ht="45.75" thickBot="1">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -882,8 +1128,16 @@
       <c r="D10" s="3">
         <v>36</v>
       </c>
+      <c r="T10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="U10" s="3">
+        <v>42.2</v>
+      </c>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:21" ht="75.75" thickBot="1">
+    <row r="11" spans="1:36" ht="75.75" thickBot="1">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -896,9 +1150,41 @@
       <c r="D11" s="3">
         <v>6849</v>
       </c>
+      <c r="T11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="U11" s="3">
+        <v>5468</v>
+      </c>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+    </row>
+    <row r="13" spans="1:36">
+      <c r="T13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="17"/>
+      <c r="AB13" s="17"/>
+      <c r="AC13" s="17"/>
+      <c r="AD13" s="17"/>
+      <c r="AE13" s="17"/>
+      <c r="AF13" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="13">
+    <mergeCell ref="AB6:AB7"/>
+    <mergeCell ref="T13:AF13"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Y6:Y7"/>
+    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="AA6:AA7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="F2:F3"/>

</xml_diff>

<commit_message>
Fixing additional HumMod lab info
</commit_message>
<xml_diff>
--- a/19_anemia/19_anemia_data.xlsx
+++ b/19_anemia/19_anemia_data.xlsx
@@ -589,7 +589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
@@ -1178,6 +1178,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
     <mergeCell ref="AB6:AB7"/>
     <mergeCell ref="T13:AF13"/>
     <mergeCell ref="T2:T3"/>
@@ -1185,12 +1191,6 @@
     <mergeCell ref="Y6:Y7"/>
     <mergeCell ref="Z6:Z7"/>
     <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>